<commit_message>
Progress on CPUE plots
</commit_message>
<xml_diff>
--- a/Data/SBOTS2019.xlsx
+++ b/Data/SBOTS2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnewe\OneDrive\Documents\Incubator\Code\FishForesightIncubator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D994276-CA1E-44EF-9685-3CF31EB494F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C40F1E-8396-4E9D-A2F4-55D5630CA68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{280D4372-98B3-4787-AE08-774B83331FEA}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{280D4372-98B3-4787-AE08-774B83331FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1390,12 +1390,22 @@
   <dimension ref="A1:DC240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="CV9" sqref="CV9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="17" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="14" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:107" x14ac:dyDescent="0.35">

</xml_diff>